<commit_message>
agregado versiones simplificadas de reglas de OpenL Tablets
</commit_message>
<xml_diff>
--- a/openl-tablets/src/main/resources/reglas/Calculo Cuotas.xlsx
+++ b/openl-tablets/src/main/resources/reglas/Calculo Cuotas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
   <si>
     <t xml:space="preserve">Environment</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">com.example.afiliacion_wrapper</t>
   </si>
   <si>
+    <t xml:space="preserve">Version no simplificada</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rules Double CalcularCuota(AfiliacionWrapper afiliado)</t>
   </si>
   <si>
@@ -43,13 +46,22 @@
     <t xml:space="preserve">RET1</t>
   </si>
   <si>
+    <t xml:space="preserve">categoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subcategoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
     <t xml:space="preserve">categoria == afiliado.getCategoria()</t>
   </si>
   <si>
     <t xml:space="preserve">subCategoria == afiliado.getSubcategoria()</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
+    <t xml:space="preserve">Double value</t>
   </si>
   <si>
     <t xml:space="preserve">String categoria</t>
@@ -58,9 +70,6 @@
     <t xml:space="preserve">String subCategoria</t>
   </si>
   <si>
-    <t xml:space="preserve">Double value</t>
-  </si>
-  <si>
     <t xml:space="preserve">Categoria</t>
   </si>
   <si>
@@ -76,6 +85,9 @@
     <t xml:space="preserve">CONYUGE</t>
   </si>
   <si>
+    <t xml:space="preserve">=CalcularCuota(conyuge) * 0.7</t>
+  </si>
+  <si>
     <t xml:space="preserve">=CalcularCuota(afiliado.getConyuge()) * 0.7</t>
   </si>
   <si>
@@ -91,6 +103,9 @@
     <t xml:space="preserve">BECARIO</t>
   </si>
   <si>
+    <t xml:space="preserve">=CMMU * ModificadorBecario(afiliado)</t>
+  </si>
+  <si>
     <t xml:space="preserve">=afiliado.getCMMU() * ModificadorBecario(afiliado)</t>
   </si>
   <si>
@@ -110,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edad</t>
   </si>
   <si>
     <t xml:space="preserve">afiliado.getEdad() &gt;= min</t>
@@ -383,7 +401,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,6 +500,42 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -501,19 +555,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G37"/>
+  <dimension ref="B2:H39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="42.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.6"/>
@@ -539,315 +593,569 @@
       <c r="G3" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="s">
+      <c r="F5" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="F7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="G8" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="H8" s="10" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="F9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="G9" s="11" t="s">
         <v>15</v>
       </c>
+      <c r="H9" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="15" t="s">
         <v>18</v>
       </c>
+      <c r="F10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="16"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>19</v>
       </c>
+      <c r="C11" s="17" t="s">
+        <v>20</v>
+      </c>
       <c r="D11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>20</v>
       </c>
+      <c r="H11" s="18" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>22</v>
+      <c r="B12" s="16"/>
+      <c r="C12" s="19" t="s">
+        <v>23</v>
       </c>
       <c r="D12" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="19" t="s">
         <v>23</v>
       </c>
+      <c r="H12" s="18" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="20"/>
+      <c r="B13" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="C13" s="21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="20" t="s">
         <v>25</v>
       </c>
+      <c r="G13" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24" t="s">
-        <v>26</v>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="F17" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="B18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="30"/>
+      <c r="C23" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D23" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21" t="n">
+        <v>30</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="30" t="n">
         <v>31</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="11" t="s">
+      <c r="C24" s="31" t="n">
+        <v>45</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="20" t="n">
+        <v>31</v>
+      </c>
+      <c r="G24" s="21" t="n">
+        <v>45</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="30" t="n">
+        <v>46</v>
+      </c>
+      <c r="C25" s="31" t="n">
+        <v>55</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="20" t="n">
+        <v>46</v>
+      </c>
+      <c r="G25" s="21" t="n">
+        <v>55</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="30" t="n">
+        <v>56</v>
+      </c>
+      <c r="C26" s="31" t="n">
+        <v>65</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F26" s="20" t="n">
+        <v>56</v>
+      </c>
+      <c r="G26" s="21" t="n">
+        <v>65</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="32" t="n">
+        <v>66</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="22" t="n">
+        <v>66</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F29" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="13" t="s">
+      <c r="C31" s="25"/>
+      <c r="D31" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="H31" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="C32" s="26"/>
+      <c r="D32" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="20"/>
-      <c r="C22" s="21" t="n">
+      <c r="G32" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="20"/>
+      <c r="C35" s="21" t="n">
         <v>30</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="20" t="n">
-        <v>31</v>
-      </c>
-      <c r="C23" s="21" t="n">
-        <v>45</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="20" t="n">
-        <v>46</v>
-      </c>
-      <c r="C24" s="21" t="n">
-        <v>55</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="20" t="n">
-        <v>56</v>
-      </c>
-      <c r="C25" s="21" t="n">
-        <v>65</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="22" t="n">
-        <v>66</v>
-      </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="9" t="s">
+      <c r="D35" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21" t="n">
         <v>30</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="20"/>
-      <c r="C33" s="21" t="n">
-        <v>30</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="20" t="n">
-        <v>31</v>
-      </c>
-      <c r="C34" s="21" t="n">
-        <v>45</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="20" t="n">
-        <v>46</v>
-      </c>
-      <c r="C35" s="21" t="n">
-        <v>55</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>45</v>
+      <c r="H35" s="18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="20" t="n">
+        <v>31</v>
+      </c>
+      <c r="C36" s="21" t="n">
+        <v>45</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="20" t="n">
+        <v>31</v>
+      </c>
+      <c r="G36" s="21" t="n">
+        <v>45</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="20" t="n">
+        <v>46</v>
+      </c>
+      <c r="C37" s="21" t="n">
+        <v>55</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="20" t="n">
+        <v>46</v>
+      </c>
+      <c r="G37" s="21" t="n">
+        <v>55</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="20" t="n">
         <v>56</v>
       </c>
-      <c r="C36" s="21" t="n">
+      <c r="C38" s="21" t="n">
         <v>65</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="22" t="n">
+      <c r="D38" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="20" t="n">
+        <v>56</v>
+      </c>
+      <c r="G38" s="21" t="n">
+        <v>65</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="22" t="n">
         <v>66</v>
       </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24" t="s">
-        <v>47</v>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="22" t="n">
+        <v>66</v>
+      </c>
+      <c r="G39" s="23"/>
+      <c r="H39" s="24" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="15">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>